<commit_message>
Main.py main method has been updated to work paint the automatas
</commit_message>
<xml_diff>
--- a/TEMPLATE.xlsx
+++ b/TEMPLATE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\El Sapo Perro\Documents\Archivos importantes\TdeA\Trabajos\Semestre 11\Compiladores e Intérpretes\Python Project\ConversorAutomatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EF9F4F-9EFA-40BC-B28B-E7477EFB042B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99591DE0-3B39-4506-A150-880B76679ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>ESTADOS</t>
   </si>
@@ -40,7 +40,10 @@
     <t>C</t>
   </si>
   <si>
-    <t>D</t>
+    <t>A,B</t>
+  </si>
+  <si>
+    <t>B,C</t>
   </si>
 </sst>
 </file>
@@ -380,15 +383,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,7 +402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>0</v>
       </c>
@@ -407,59 +410,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6">
         <v>1</v>
       </c>
     </row>

</xml_diff>